<commit_message>
Corrige parámetros de entrada en funciones
</commit_message>
<xml_diff>
--- a/conversor_nominas_bancos_chile/planillas_test/datos_empresas.xlsx
+++ b/conversor_nominas_bancos_chile/planillas_test/datos_empresas.xlsx
@@ -242,8 +242,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6:F8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -433,6 +433,7 @@
         <v>33</v>
       </c>
     </row>
+    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -467,7 +468,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="F6:F8 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>